<commit_message>
Added Registration Test Case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestRunmodes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>TCID</t>
   </si>
@@ -27,15 +27,9 @@
     <t>Y</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>loginTest</t>
   </si>
   <si>
-    <t>ChangePassTest</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -48,13 +42,40 @@
     <t>tester1234</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>Browser</t>
   </si>
   <si>
     <t>Mozilla</t>
+  </si>
+  <si>
+    <t>registerTest</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>testdoc14junebus@mailinator.com</t>
+  </si>
+  <si>
+    <t>Test Doc 14</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>High Street</t>
   </si>
 </sst>
 </file>
@@ -113,11 +134,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -422,13 +444,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -442,7 +464,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -450,10 +472,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -464,56 +486,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>7755114455</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="H7" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Create Contract Test Casse
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView windowWidth="19890" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestRunmodes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -24,10 +24,19 @@
     <t>Runmode</t>
   </si>
   <si>
+    <t>loginTest</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>loginTest</t>
+    <t>registerTest</t>
+  </si>
+  <si>
+    <t>changePasswordTest</t>
+  </si>
+  <si>
+    <t>createcontractTest</t>
   </si>
   <si>
     <t>UserName</t>
@@ -36,21 +45,18 @@
     <t>Password</t>
   </si>
   <si>
+    <t>Browser</t>
+  </si>
+  <si>
     <t>testdoc1jan@mailinator.com</t>
   </si>
   <si>
     <t>tester1234</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>Mozilla</t>
   </si>
   <si>
-    <t>registerTest</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -66,28 +72,101 @@
     <t>Address</t>
   </si>
   <si>
+    <t>Test Doc 14</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
     <t>testdoc14junebus@mailinator.com</t>
   </si>
   <si>
-    <t>Test Doc 14</t>
-  </si>
-  <si>
-    <t>June</t>
-  </si>
-  <si>
     <t>High Street</t>
+  </si>
+  <si>
+    <t>changepasswordTest</t>
+  </si>
+  <si>
+    <t>CurrentPassword</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>ConfirmNewPassword</t>
+  </si>
+  <si>
+    <t>tester12345</t>
+  </si>
+  <si>
+    <t>ContractType</t>
+  </si>
+  <si>
+    <t>ServiceCost</t>
+  </si>
+  <si>
+    <t>DownPayment</t>
+  </si>
+  <si>
+    <t>CustomerEmail</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>CusFirstName</t>
+  </si>
+  <si>
+    <t>CusLastName</t>
+  </si>
+  <si>
+    <t>CusSSN</t>
+  </si>
+  <si>
+    <t>CusPhone</t>
+  </si>
+  <si>
+    <t>CusDL</t>
+  </si>
+  <si>
+    <t>CusAddress</t>
+  </si>
+  <si>
+    <t>CusZip</t>
+  </si>
+  <si>
+    <t>EmpName</t>
+  </si>
+  <si>
+    <t>EmpPhone</t>
+  </si>
+  <si>
+    <t>EmpAddress</t>
+  </si>
+  <si>
+    <t>EmpZip</t>
+  </si>
+  <si>
+    <t>testpatient14july@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd/mmm"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -95,7 +174,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -103,11 +182,154 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,8 +342,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -129,23 +537,309 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -436,25 +1130,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="9.57142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,154 +1156,308 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="14.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="22.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="35.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="14.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="13.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="10.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="10.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="6.85714285714286" customWidth="1"/>
+    <col min="11" max="11" width="12.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="7.42857142857143" customWidth="1"/>
+    <col min="13" max="13" width="10.8571428571429" customWidth="1"/>
+    <col min="14" max="14" width="11.2857142857143" customWidth="1"/>
+    <col min="15" max="15" width="12.8571428571429" customWidth="1"/>
+    <col min="16" max="16" width="8.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C7">
         <v>7755114455</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" spans="1:18">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
         <v>2</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId1" display="testdoc1jan@mailinator.com"/>
+    <hyperlink ref="D7" r:id="rId2" display="testdoc14junebus@mailinator.com"/>
+    <hyperlink ref="F15" r:id="rId3" display="testpatient14july@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>